<commit_message>
fixed 12v aux bootstrap capacitor
bootstrap capacitor connected after inductor originally, now changed to be connected to switch node.
</commit_message>
<xml_diff>
--- a/powersystem/vrm/hardware/Default Configuration/Outputs/BOM/BOM_PartType-vrm.xlsx
+++ b/powersystem/vrm/hardware/Default Configuration/Outputs/BOM/BOM_PartType-vrm.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E985302-EE83-4B95-8CE0-4B0157976163}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{13B9DBC4-6E23-4194-B271-2B8BCDEC7DBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16423" windowHeight="8289" xr2:uid="{7728DBF0-8A93-4B4E-90B1-820049069426}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24669" windowHeight="12257" xr2:uid="{CAEF9E4E-B718-497E-AA77-39D92A6305E5}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-vrm" sheetId="1" r:id="rId1"/>
@@ -971,7 +971,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8014A3-9E1D-4E10-9E6F-E70071B9FCA0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC68A9A7-868D-43D9-B60E-0C6B2E2317EE}">
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
remove enable transistor on 12V Main PSU
Turns out this isn't needed - on further consultation of the datasheet it can be driven directly from the microcontroller pin, although it is right on the limit of the threshold. This may cause problems in future but experimental testing shows that it works.
</commit_message>
<xml_diff>
--- a/powersystem/vrm/hardware/Default Configuration/Outputs/BOM/BOM_PartType-vrm.xlsx
+++ b/powersystem/vrm/hardware/Default Configuration/Outputs/BOM/BOM_PartType-vrm.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13B9DBC4-6E23-4194-B271-2B8BCDEC7DBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{95094D79-8D41-4445-8C1A-00E1111F63BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24669" windowHeight="12257" xr2:uid="{CAEF9E4E-B718-497E-AA77-39D92A6305E5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="8508" xr2:uid="{7F9E482C-B278-42AC-A9C3-7E5DBE979969}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-vrm" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="182">
   <si>
     <t>Description</t>
   </si>
@@ -318,18 +318,6 @@
     <t>CSD19534Q5A</t>
   </si>
   <si>
-    <t>P-CHANNEL ENHANCEMENT MODE MOSFET</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>Diodes Incorporated</t>
-  </si>
-  <si>
-    <t>DMG2307L</t>
-  </si>
-  <si>
     <t>100V POWERTRENCH N-ch MOSFET</t>
   </si>
   <si>
@@ -342,178 +330,172 @@
     <t>FDWS86068-F085</t>
   </si>
   <si>
-    <t>100K 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R1</t>
+    <t>86K6 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>86K6</t>
+  </si>
+  <si>
+    <t>3K4 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>3K4</t>
+  </si>
+  <si>
+    <t>10K 0.1W 5% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R4, R33, R34</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>R5, R9, R17</t>
+  </si>
+  <si>
+    <t>Susumu</t>
+  </si>
+  <si>
+    <t>5mR</t>
+  </si>
+  <si>
+    <t>56K 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R6, R19</t>
+  </si>
+  <si>
+    <t>56K</t>
+  </si>
+  <si>
+    <t>23K7 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>23K7</t>
+  </si>
+  <si>
+    <t>9K76 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>9K76</t>
+  </si>
+  <si>
+    <t>28K 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>28K</t>
+  </si>
+  <si>
+    <t>220R 0.1W 5% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R11, R22, R28, R29, R30, R31, R32, R35</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>1K1 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>1K1</t>
+  </si>
+  <si>
+    <t>10K 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R13, R18, R23</t>
+  </si>
+  <si>
+    <t>464K 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>464K</t>
+  </si>
+  <si>
+    <t>301K 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>301K</t>
+  </si>
+  <si>
+    <t>78K7 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>78K7</t>
+  </si>
+  <si>
+    <t>2K74 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>2K74</t>
+  </si>
+  <si>
+    <t>2K 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>2K</t>
+  </si>
+  <si>
+    <t>61K9 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>61K9</t>
+  </si>
+  <si>
+    <t>20K5 0.1W 1% 0603 (1608 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>20K5</t>
+  </si>
+  <si>
+    <t>100K 0.125W 1% 0805 (2012 Metric)  SMD</t>
+  </si>
+  <si>
+    <t>R26</t>
   </si>
   <si>
     <t>100K</t>
-  </si>
-  <si>
-    <t>86K6 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>86K6</t>
-  </si>
-  <si>
-    <t>3K4 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>3K4</t>
-  </si>
-  <si>
-    <t>10K 0.1W 5% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R4, R33, R34</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>R5, R9, R17</t>
-  </si>
-  <si>
-    <t>Susumu</t>
-  </si>
-  <si>
-    <t>5mR</t>
-  </si>
-  <si>
-    <t>56K 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R6, R19</t>
-  </si>
-  <si>
-    <t>56K</t>
-  </si>
-  <si>
-    <t>23K7 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>23K7</t>
-  </si>
-  <si>
-    <t>9K76 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>9K76</t>
-  </si>
-  <si>
-    <t>28K 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>28K</t>
-  </si>
-  <si>
-    <t>220R 0.1W 5% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R11, R22, R28, R29, R30, R31, R32, R35</t>
-  </si>
-  <si>
-    <t>220R</t>
-  </si>
-  <si>
-    <t>1K1 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>1K1</t>
-  </si>
-  <si>
-    <t>10K 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R13, R18, R23</t>
-  </si>
-  <si>
-    <t>464K 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>464K</t>
-  </si>
-  <si>
-    <t>301K 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>301K</t>
-  </si>
-  <si>
-    <t>78K7 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>78K7</t>
-  </si>
-  <si>
-    <t>2K74 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>2K74</t>
-  </si>
-  <si>
-    <t>2K 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>2K</t>
-  </si>
-  <si>
-    <t>61K9 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>61K9</t>
-  </si>
-  <si>
-    <t>20K5 0.1W 1% 0603 (1608 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R25</t>
-  </si>
-  <si>
-    <t>20K5</t>
-  </si>
-  <si>
-    <t>100K 0.125W 1% 0805 (2012 Metric)  SMD</t>
-  </si>
-  <si>
-    <t>R26</t>
   </si>
   <si>
     <t>2K7 0.125W 1% 0805 (2012 Metric)  SMD</t>
@@ -971,19 +953,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC68A9A7-868D-43D9-B60E-0C6B2E2317EE}">
-  <dimension ref="A1:G62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D304C00-FFCD-47E2-ADBE-C77EDE8393CC}">
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="28.23046875" customWidth="1"/>
-    <col min="2" max="6" width="7.53515625" customWidth="1"/>
-    <col min="7" max="7" width="7.3828125" customWidth="1"/>
+    <col min="1" max="1" width="29.578125" customWidth="1"/>
+    <col min="2" max="6" width="7.734375" customWidth="1"/>
+    <col min="7" max="7" width="7.62890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1029,7 +1011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1052,7 +1034,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1075,7 +1057,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -1098,7 +1080,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1121,7 +1103,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1144,7 +1126,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -1167,7 +1149,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
@@ -1190,7 +1172,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
@@ -1213,7 +1195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1236,7 +1218,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1259,7 +1241,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
@@ -1282,7 +1264,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
         <v>45</v>
       </c>
@@ -1305,7 +1287,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
         <v>47</v>
       </c>
@@ -1328,7 +1310,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1351,7 +1333,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
         <v>53</v>
       </c>
@@ -1374,7 +1356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
         <v>56</v>
       </c>
@@ -1397,7 +1379,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
         <v>59</v>
       </c>
@@ -1420,7 +1402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
         <v>61</v>
       </c>
@@ -1443,7 +1425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -1466,7 +1448,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -1489,7 +1471,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
         <v>71</v>
       </c>
@@ -1512,7 +1494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
         <v>73</v>
       </c>
@@ -1535,7 +1517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
         <v>75</v>
       </c>
@@ -1558,7 +1540,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
         <v>79</v>
       </c>
@@ -1581,7 +1563,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
@@ -1604,7 +1586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
         <v>85</v>
       </c>
@@ -1627,7 +1609,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
         <v>88</v>
       </c>
@@ -1650,7 +1632,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
         <v>91</v>
       </c>
@@ -1673,7 +1655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
         <v>93</v>
       </c>
@@ -1696,7 +1678,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
         <v>97</v>
       </c>
@@ -1710,7 +1692,7 @@
         <v>9</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="F32" s="3">
         <v>1</v>
@@ -1719,7 +1701,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
         <v>101</v>
       </c>
@@ -1727,482 +1709,482 @@
         <v>102</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F33" s="3">
-        <v>1</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="3">
+        <v>1</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="3">
-        <v>1</v>
-      </c>
-      <c r="G34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A35" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="3">
+        <v>3</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="3">
-        <v>1</v>
-      </c>
-      <c r="G35" s="2" t="s">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="D36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="3">
+        <v>3</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="3">
-        <v>1</v>
-      </c>
-      <c r="G36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A37" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="3">
+        <v>2</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="3">
-        <v>3</v>
-      </c>
-      <c r="G37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="2" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="3">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="3">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="3">
+        <v>1</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="3">
+        <v>8</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="3">
+        <v>1</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="3">
         <v>3</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A39" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="3">
-        <v>2</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A40" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="3">
-        <v>1</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A41" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="3">
-        <v>1</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A42" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="3">
-        <v>1</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A43" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B43" s="2" t="s">
+      <c r="G43" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="3">
-        <v>8</v>
-      </c>
-      <c r="G43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A44" s="2" t="s">
+      <c r="C44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="3">
+        <v>1</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="2" t="s">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="3">
-        <v>1</v>
-      </c>
-      <c r="G44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A45" s="2" t="s">
+      <c r="C45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="3">
+        <v>1</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B45" s="2" t="s">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="3">
-        <v>3</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A46" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1</v>
+      </c>
+      <c r="G46" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="3">
-        <v>1</v>
-      </c>
-      <c r="G46" s="2" t="s">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A47" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="3">
+        <v>1</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="3">
-        <v>1</v>
-      </c>
-      <c r="G47" s="2" t="s">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A48" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="3">
+        <v>1</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="3">
-        <v>1</v>
-      </c>
-      <c r="G48" s="2" t="s">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A49" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="3">
+        <v>1</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="3">
-        <v>1</v>
-      </c>
-      <c r="G49" s="2" t="s">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A50" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="3">
+        <v>1</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="3">
-        <v>1</v>
-      </c>
-      <c r="G50" s="2" t="s">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A51" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="3">
+        <v>1</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="3">
-        <v>1</v>
-      </c>
-      <c r="G51" s="2" t="s">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A52" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="3">
+        <v>1</v>
+      </c>
+      <c r="G52" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="3">
-        <v>1</v>
-      </c>
-      <c r="G52" s="2" t="s">
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A53" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="3">
+        <v>1</v>
+      </c>
+      <c r="G53" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="3">
-        <v>1</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2" t="s">
         <v>163</v>
       </c>
@@ -2210,7 +2192,7 @@
         <v>164</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>9</v>
@@ -2222,38 +2204,38 @@
         <v>1</v>
       </c>
       <c r="G54" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A55" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="3">
+        <v>2</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="3">
-        <v>1</v>
-      </c>
-      <c r="G55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A56" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>95</v>
@@ -2262,16 +2244,16 @@
         <v>9</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>9</v>
+        <v>169</v>
       </c>
       <c r="F56" s="3">
         <v>1</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2" t="s">
         <v>171</v>
       </c>
@@ -2288,36 +2270,36 @@
         <v>9</v>
       </c>
       <c r="F57" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>175</v>
+        <v>9</v>
       </c>
       <c r="F58" s="3">
         <v>1</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2" t="s">
         <v>177</v>
       </c>
@@ -2337,19 +2319,19 @@
         <v>1</v>
       </c>
       <c r="G59" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A60" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="D60" s="2" t="s">
         <v>9</v>
       </c>
@@ -2360,52 +2342,6 @@
         <v>1</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A61" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="3">
-        <v>1</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A62" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="3">
-        <v>1</v>
-      </c>
-      <c r="G62" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
connect LM5116 pin 17 to GND
TI datasheet says to connect pin 17 to ground if not using external VCC, added via and connected to ground.
</commit_message>
<xml_diff>
--- a/powersystem/vrm/hardware/Default Configuration/Outputs/BOM/BOM_PartType-vrm.xlsx
+++ b/powersystem/vrm/hardware/Default Configuration/Outputs/BOM/BOM_PartType-vrm.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95094D79-8D41-4445-8C1A-00E1111F63BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCCB2283-50D3-457B-A2D6-D57F2C54B8E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="8508" xr2:uid="{7F9E482C-B278-42AC-A9C3-7E5DBE979969}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="8508" xr2:uid="{78B09034-9DD2-4E9E-AB04-671129174D6F}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-vrm" sheetId="1" r:id="rId1"/>
@@ -953,7 +953,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D304C00-FFCD-47E2-ADBE-C77EDE8393CC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD2E9E4-8350-4F23-8366-94ADA2CBC2E9}">
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>